<commit_message>
Pivotal-155067936: Add Json submission integration test https://www.pivotaltracker.com/story/show/155067936 - added json integration test - minor improvements in dependency managment and formating
</commit_message>
<xml_diff>
--- a/BackendWebApp/src/test/resources/input/S-BSST56.pagetab_for_test.xlsx
+++ b/BackendWebApp/src/test/resources/input/S-BSST56.pagetab_for_test.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Submission</t>
   </si>
   <si>
-    <t xml:space="preserve">S-ACC-TEST</t>
+    <t xml:space="preserve">S-ACC-TEST-XLSX</t>
   </si>
   <si>
     <t xml:space="preserve">Public</t>
@@ -141,6 +141,7 @@
       <sz val="11.5"/>
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,7 +219,7 @@
   <dimension ref="A2:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Pivotal-155067936: Add Json submission integration test (#16)
* Pivotal-155067936: Add Json submission integration test
https://www.pivotaltracker.com/story/show/155067936
- added json integration test
- minor improvements in dependency managment and formating
</commit_message>
<xml_diff>
--- a/BackendWebApp/src/test/resources/input/S-BSST56.pagetab_for_test.xlsx
+++ b/BackendWebApp/src/test/resources/input/S-BSST56.pagetab_for_test.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Submission</t>
   </si>
   <si>
-    <t xml:space="preserve">S-ACC-TEST</t>
+    <t xml:space="preserve">S-ACC-TEST-XLSX</t>
   </si>
   <si>
     <t xml:space="preserve">Public</t>
@@ -141,6 +141,7 @@
       <sz val="11.5"/>
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,7 +219,7 @@
   <dimension ref="A2:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>